<commit_message>
Update file with new data
</commit_message>
<xml_diff>
--- a/test_git.xlsx
+++ b/test_git.xlsx
@@ -1,26 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FRACK004\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD67585-CB64-48D3-9155-E28715E68CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -36,9 +25,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -54,7 +51,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,26 +59,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -96,44 +103,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -160,15 +167,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -195,7 +201,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -207,164 +212,186 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -372,7 +399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -380,7 +407,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -388,7 +415,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -396,11 +423,51 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
         <v>5</v>
       </c>
     </row>

</xml_diff>